<commit_message>
Added new test files and updated POM
</commit_message>
<xml_diff>
--- a/playwrightTestingPractice/testcases/test_results1.xlsx
+++ b/playwrightTestingPractice/testcases/test_results1.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$21.00</t>
+          <t>$61.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/13/2026</t>
+          <t>01/20/2026</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -481,12 +481,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$171.00</t>
+          <t>$31.50</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/13/2026</t>
+          <t>01/19/2026</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -501,12 +501,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$21.00</t>
+          <t>$185.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/12/2026</t>
+          <t>01/19/2026</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -521,12 +521,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$21.00</t>
+          <t>$129.00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/12/2026</t>
+          <t>01/19/2026</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -541,12 +541,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$21.00</t>
+          <t>$110.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/12/2026</t>
+          <t>01/19/2026</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -561,12 +561,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$69.50</t>
+          <t>$48.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/12/2026</t>
+          <t>01/13/2026</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -581,12 +581,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$69.50</t>
+          <t>$21.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/12/2026</t>
+          <t>01/13/2026</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -597,10 +597,14 @@
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>$171.00</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/12/2026</t>
+          <t>01/13/2026</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -611,7 +615,11 @@
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>$21.00</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>01/12/2026</t>
@@ -625,7 +633,11 @@
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>$21.00</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>01/12/2026</t>
@@ -639,7 +651,11 @@
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>$21.00</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>01/12/2026</t>
@@ -653,7 +669,11 @@
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>$69.50</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>01/12/2026</t>
@@ -667,7 +687,11 @@
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>$69.50</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>01/12/2026</t>
@@ -681,7 +705,11 @@
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>$31.50</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>01/12/2026</t>
@@ -695,10 +723,14 @@
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>$195.50</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01/11/2026</t>
+          <t>01/12/2026</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -709,10 +741,14 @@
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>$106.50</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01/11/2026</t>
+          <t>01/12/2026</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -723,10 +759,14 @@
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>$77.00</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01/11/2026</t>
+          <t>01/12/2026</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -737,10 +777,14 @@
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>$21.00</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/11/2026</t>
+          <t>01/12/2026</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -751,10 +795,14 @@
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>$21.00</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>12/31/2025</t>
+          <t>01/12/2026</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -765,10 +813,14 @@
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>$21.00</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>12/31/2025</t>
+          <t>01/12/2026</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>